<commit_message>
panel annotation family and some refinement
</commit_message>
<xml_diff>
--- a/Curtain_Schedule.xlsx
+++ b/Curtain_Schedule.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C1F38F-47EC-4D7B-AC7F-1CAB596DC64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFE792A-957D-4E82-836C-70FD30E599F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24015" yWindow="5595" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -733,7 +733,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2661ABEC-DC5A-435E-A638-F01FA180EB9D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CF026F5-4B94-4ED5-A8D7-4C3C6DE79E8F}">
   <dimension ref="A2:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>